<commit_message>
commit 21012025 F3 mappings
</commit_message>
<xml_diff>
--- a/Inputs/PyDump.xlsx
+++ b/Inputs/PyDump.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M327220\Documents\GitHub\GCOHFilesTicketsEtc\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47925751-1B8E-4C42-861A-B7053C052386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5972DA-FCBE-47B4-BCB4-16D577CB08E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6A12B107-397F-4BA6-8F78-4BB99A484E33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{6A12B107-397F-4BA6-8F78-4BB99A484E33}"/>
   </bookViews>
   <sheets>
     <sheet name="Dump" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Object</t>
   </si>
@@ -79,6 +79,75 @@
   </si>
   <si>
     <t>L000013318</t>
+  </si>
+  <si>
+    <t>D00123500000000 AP5008</t>
+  </si>
+  <si>
+    <t>P000001013</t>
+  </si>
+  <si>
+    <t>D00118900000000 Ultra-High Purity Colloidal Silica PD Su</t>
+  </si>
+  <si>
+    <t>D00123000000000 Optiplane 2260</t>
+  </si>
+  <si>
+    <t>DP000010000000 Cu3886 low dishing low defect Cu Bulk Sl</t>
+  </si>
+  <si>
+    <t>P000001016</t>
+  </si>
+  <si>
+    <t>D00123300000000 Str Partnership IMEC TFM Share</t>
+  </si>
+  <si>
+    <t>P000001012</t>
+  </si>
+  <si>
+    <t>D00123200000000 Adv Pkg CMP (1501-50 BOOST)</t>
+  </si>
+  <si>
+    <t>D00115200000000 Ultra-High Purity Colloidal Silica</t>
+  </si>
+  <si>
+    <t>DP000005000000 DP1284 high-rate Cu bulk slurry for TI</t>
+  </si>
+  <si>
+    <t>RD210008 Advanced particle characterization</t>
+  </si>
+  <si>
+    <t>RD242007 HPD8700 for Micron HBM CMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPHOENX_01010000604520 </t>
+  </si>
+  <si>
+    <t>L000010145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPHOENX_01010000604540 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPHOENX_01010000604530 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORAERP_MMOR1975.4147 </t>
+  </si>
+  <si>
+    <t>L000009822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEMPEU_001300003829 </t>
+  </si>
+  <si>
+    <t>L000013174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORAERP_MMOR1975.SMQA </t>
+  </si>
+  <si>
+    <t>L000006414</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1231,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9544D389-BCBF-4017-8282-1DF88DB28091}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1184,49 +1253,177 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B23" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>